<commit_message>
Excell Reader and SpeedTester Logic completion
DEscriçao
</commit_message>
<xml_diff>
--- a/Files/FibraOticaExcell.xlsx
+++ b/Files/FibraOticaExcell.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Nome</t>
   </si>
@@ -19,10 +19,7 @@
     <t>Problema</t>
   </si>
   <si>
-    <t>as</t>
-  </si>
-  <si>
-    <t>asssss</t>
+    <t>Idade</t>
   </si>
 </sst>
 </file>
@@ -288,13 +285,8 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>